<commit_message>
Created CDS TC01,2 for Acesses
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Acesses-Controlled.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Acesses-Controlled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5BBDB6-B358-4869-86EA-AF1C0B3799A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A01967-22C2-4F03-B6BB-B4A7C13D0C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,89 +55,6 @@
   </si>
   <si>
     <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-  MATCH (demo:demographic) 
-  MATCH (diag:diagnosis)
- MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-	WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
-OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case)
-OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)&lt;-[:of_sample]-(f:file)
-RETURN 
-	count(DISTINCT(f)) as number_of_files , 
-	count(DISTINCT(samp)) as number_of_sample , 
-	count(DISTINCT(c.case_id)) as number_of_cases , 
-	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
-WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
- WITH DISTINCT samp AS samp, c, demo, diag
-RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(samp.sample_site, '') AS `Sample Site`,
-        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
-        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
-        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
-        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
-        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
-        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(f.file_type, '') AS `File Type`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `File Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-  MATCH (demo:demographic) 
-  MATCH (diag:diagnosis)
- MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-	WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
-OPTIONAL MATCH (s)&lt;-[:member_of]-(c:case)
-OPTIONAL MATCH (c)&lt;-[:of_case]-(samp:sample)&lt;-[:of_sample]-(f:file)
-RETURN 
-	count(DISTINCT(f)) as number_of_files , 
-	count(DISTINCT(samp)) as number_of_sample , 
-	count(DISTINCT(c.case_id)) as number_of_cases , 
-	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['MGT01'] and demo.breed in ['Australian Cattle Dog','Mixed Breed']and diag.disease_term in ['Mammary Cancer'] and diag.primary_disease_site in ['Mammary Gland']
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
   <si>
     <t>TC01_CDS_Filter_Acesses-Controlled_WebData.xlsx</t>
@@ -516,7 +433,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,55 +461,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added queries to CDS tests
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Acesses-Controlled.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Acesses-Controlled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A01967-22C2-4F03-B6BB-B4A7C13D0C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8CADE2-1626-4DA2-834E-6A617E27A8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>WebExcel</t>
   </si>
@@ -61,13 +61,88 @@
   </si>
   <si>
     <t>TC01_CDS_Filter_Acesses-Controlled_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE s.data_access_level in ["controlled"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p
+RETURN  
+ coalesce(p.participant_id,'') as `Case ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+ coalesce(samp.sample_anatomic_site,'') as `Site`,
+ coalesce(samp.sample_id, '') as `Samples`
+ ORDER By p.participant_id</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p,f
+WHERE s.data_access_level in ["controlled"]
+RETURN
+    count(distinct s) AS Studies,
+    count(distinct diag.primary_diagnosis) AS `Disease Sites`,
+    count(distinct p) AS Participants,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE s.data_access_level in ["controlled"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p
+RETURN  
+ coalesce(samp.sample_id, '') as `Sample ID` ,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(samp.sample_tumor_status,'') as `Tumor`,
+coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER By samp.sample_id</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE s.data_access_level in ["controlled"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT p,s,samp,f,diag
+RETURN 
+    coalesce(f.file_name, '') as `File Name`,
+    coalesce(s.study_name, '') as `Study Name`,
+    coalesce(s.phs_accession,'') as `Accession`,
+    coalesce(p.participant_id,'') as `Subject ID`,
+    coalesce(samp.sample_id, '') as `Sample ID`,
+    coalesce(f.file_type, '') as `File Type`
+   ORDER By f.file_name</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p,f
+WHERE s.study_name in ["CDS-Study-A"]
+RETURN
+    count(distinct s) AS Studies,
+    count(distinct diag.primary_diagnosis) AS `Disease Sites`,
+    count(distinct p) AS Participants,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Files`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +159,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,9 +192,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,7 +518,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,12 +546,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -474,12 +563,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="234" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
@@ -487,12 +580,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="218.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>

</xml_diff>